<commit_message>
new doc and updated html
</commit_message>
<xml_diff>
--- a/Groupwork/DF final.xlsx
+++ b/Groupwork/DF final.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="138" documentId="8_{0BFD528B-9ABF-4C8F-89A1-F1492E273C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2DC2404-0939-48B4-A1F9-A761DE1F7C07}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="75" windowWidth="16200" windowHeight="9308" firstSheet="5" activeTab="5" xr2:uid="{710F251B-32F8-40FC-8DC3-610372DBFCD8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{710F251B-32F8-40FC-8DC3-610372DBFCD8}"/>
   </bookViews>
   <sheets>
     <sheet name="PRICES" sheetId="2" r:id="rId1"/>
@@ -42572,8 +42572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883ADA5E-0EC8-4F04-AFF2-AC3EAF4C7307}">
   <dimension ref="A1:AX110"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="84" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -48830,7 +48830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19277D1A-0DFC-4D8C-8B47-C6F58CB8D264}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>